<commit_message>
modbus debug + updated sw matrix files
</commit_message>
<xml_diff>
--- a/flexlab/sw_mat_HIL2/HIL2_switch_matrix_13NF_bal.xlsx
+++ b/flexlab/sw_mat_HIL2/HIL2_switch_matrix_13NF_bal.xlsx
@@ -93,10 +93,10 @@
     <t>sw_Inverter_A_to_692_A</t>
   </si>
   <si>
-    <t>Flexgrid PV scale</t>
-  </si>
-  <si>
-    <t>Loadrack scale</t>
+    <t>scale_flexgrid PV</t>
+  </si>
+  <si>
+    <t>scale_loadrack</t>
   </si>
   <si>
     <t>Loadrack_P_A</t>
@@ -206,7 +206,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,7 +215,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="9"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -243,6 +243,12 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="15"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -254,35 +260,35 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top/>
@@ -299,39 +305,39 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -348,35 +354,20 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
@@ -384,31 +375,46 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -417,10 +423,10 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -440,6 +446,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="fff4cccc"/>
       <rgbColor rgb="ffb6d7a8"/>
@@ -644,17 +651,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -682,10 +689,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -933,12 +940,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1225,7 +1232,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1253,10 +1260,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">

</xml_diff>

<commit_message>
13bal sw mat, scale update to 7500
</commit_message>
<xml_diff>
--- a/flexlab/sw_mat_HIL2/HIL2_switch_matrix_13NF_bal.xlsx
+++ b/flexlab/sw_mat_HIL2/HIL2_switch_matrix_13NF_bal.xlsx
@@ -2196,34 +2196,34 @@
         <v>26</v>
       </c>
       <c r="C16" s="15">
-        <v>2273</v>
+        <v>7500</v>
       </c>
       <c r="D16" s="15">
-        <v>2273</v>
+        <v>7500</v>
       </c>
       <c r="E16" s="15">
-        <v>2273</v>
+        <v>7500</v>
       </c>
       <c r="F16" s="15">
-        <v>2273</v>
+        <v>7500</v>
       </c>
       <c r="G16" s="15">
-        <v>2273</v>
+        <v>7500</v>
       </c>
       <c r="H16" s="15">
-        <v>2273</v>
+        <v>7500</v>
       </c>
       <c r="I16" s="15">
-        <v>2273</v>
+        <v>7500</v>
       </c>
       <c r="J16" s="15">
-        <v>2273</v>
+        <v>7500</v>
       </c>
       <c r="K16" s="15">
-        <v>2273</v>
+        <v>7500</v>
       </c>
       <c r="L16" s="15">
-        <v>2273</v>
+        <v>7500</v>
       </c>
       <c r="M16" s="16"/>
       <c r="N16" s="16"/>

</xml_diff>